<commit_message>
grades-0.8.xsd development and documentation (white paper). State: WIP.
</commit_message>
<xml_diff>
--- a/gradinghints/images/images.xlsx
+++ b/gradinghints/images/images.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="4515" windowHeight="6225" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="4515" windowHeight="6225"/>
   </bookViews>
   <sheets>
     <sheet name="Example1a" sheetId="1" r:id="rId1"/>
@@ -256,9 +256,6 @@
     <t>Printing instructions:</t>
   </si>
   <si>
-    <t>convert images.tif -trim whitepaper-grades-example-img.png</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">* Print to </t>
     </r>
@@ -320,13 +317,16 @@
   <si>
     <t>▶ 2.27</t>
   </si>
+  <si>
+    <t>convert images.tif -trim -geometry 600x whitepaper-grades-example-img.png</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.00\ \ &quot; ⓘ&quot;"/>
+    <numFmt numFmtId="164" formatCode="0.00\ \ &quot; ⓘ&quot;"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -503,6 +503,20 @@
   </cellStyleXfs>
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -515,33 +529,82 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -549,69 +612,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -916,7 +916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -929,72 +929,72 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="13"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="9" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="9" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
@@ -1003,17 +1003,17 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="38" t="s">
-        <v>51</v>
+      <c r="C16" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1050,129 +1050,132 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="13" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="13"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="22" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="22"/>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="6"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="2:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="36" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="6"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="22"/>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="6"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="2:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="36" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="37"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="6"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="22" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="22"/>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="6"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="36" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="6"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="22" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="22"/>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="36" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="6"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E7:F7"/>
     <mergeCell ref="B4:B12"/>
     <mergeCell ref="G4:G12"/>
     <mergeCell ref="B2:D2"/>
@@ -1189,9 +1192,6 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1217,203 +1217,216 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="13" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="6"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27" t="s">
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="6"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="34" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="6"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="22" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="22"/>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="6"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="35" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="6"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="31"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="22" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="22"/>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="6"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="35" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="6"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="26" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="30" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="6"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="34" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="6"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="31"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="22" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="22"/>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="6"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="35" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="6"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="13"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="31"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="22" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="22"/>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="6"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="13"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="35" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="6"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:B16"/>
+    <mergeCell ref="I4:I16"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="D6:G6"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="F11:H11"/>
@@ -1430,19 +1443,6 @@
     <mergeCell ref="H6:H10"/>
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:B16"/>
-    <mergeCell ref="I4:I16"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1468,203 +1468,216 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="13" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="6"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="30" t="s">
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="6"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="34" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="6"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="22" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="22"/>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="6"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="2:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="35" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="6"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="31"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="22" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="22"/>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="6"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="2:9" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="35" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="6"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="26" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="30" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="6"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="2:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="34" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="6"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="31"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="22" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="22"/>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="6"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="35" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="6"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="13"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="31"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="22" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="22"/>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="6"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="13"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="35" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="6"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:B16"/>
+    <mergeCell ref="I4:I16"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:C10"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="C4:H4"/>
     <mergeCell ref="C11:E11"/>
@@ -1681,19 +1694,6 @@
     <mergeCell ref="H6:H10"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:B16"/>
-    <mergeCell ref="I4:I16"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1719,229 +1719,245 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="13" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="6"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27" t="s">
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="6"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="34" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="6"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="22" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="22"/>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="6"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="35" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="6"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="31"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="22" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="22"/>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="6"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="35" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="6"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="26" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="30" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="6"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="34" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="6"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="31"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="22" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="22"/>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="6"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="36" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="37"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="6"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="13"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="16" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="14" t="s">
+      <c r="E15" s="38"/>
+      <c r="F15" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="6"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="13"/>
     </row>
     <row r="16" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="36" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="6"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="13"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="16" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="14" t="s">
+      <c r="E17" s="38"/>
+      <c r="F17" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="6"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="13"/>
     </row>
     <row r="18" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="36" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="6"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:B18"/>
+    <mergeCell ref="I4:I18"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="H6:H10"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:G13"/>
@@ -1958,22 +1974,6 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:H10"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:B18"/>
-    <mergeCell ref="I4:I18"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1999,229 +1999,247 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="13" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="6"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27" t="s">
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="6"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="2:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="34" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="6"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="31"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="22" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="22"/>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="6"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="2:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="35" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="6"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="31"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="22" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="22"/>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="6"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="2:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="35" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="6"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="26" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="30" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="6"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="34" t="s">
+      <c r="B12" s="13"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="6"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="31"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="27"/>
       <c r="D13" s="22" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="22"/>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="6"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="36" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="37"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="6"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="13"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="16" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="14" t="s">
+      <c r="E15" s="38"/>
+      <c r="F15" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="6"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="13"/>
     </row>
     <row r="16" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="36" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="6"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="13"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="16" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="14" t="s">
+      <c r="E17" s="38"/>
+      <c r="F17" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="15"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="6"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="13"/>
     </row>
     <row r="18" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="36" t="s">
+      <c r="B18" s="13"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="6"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:B18"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="I4:I18"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:H10"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="F17:G17"/>
@@ -2236,24 +2254,6 @@
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:H10"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:B18"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="I4:I18"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2264,8 +2264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2279,138 +2279,129 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="13"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="22" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="22"/>
-      <c r="E5" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="6"/>
+      <c r="E5" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="21"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="2:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="6"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="22"/>
-      <c r="E7" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="6"/>
+      <c r="E7" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="2:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="37"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="6"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="22" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="22"/>
-      <c r="E9" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="6"/>
+      <c r="E9" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="2:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="6"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="22" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="22"/>
-      <c r="E11" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="6"/>
+      <c r="E11" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="2:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="6"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="D10:E10"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="B3:D3"/>
@@ -2421,6 +2412,15 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="D10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>